<commit_message>
FTL Xpath Changes and New extent Reports
</commit_message>
<xml_diff>
--- a/Resources/VF_Buyer_Quote_Creation.xlsx
+++ b/Resources/VF_Buyer_Quote_Creation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\workspace\VF_Hybrid\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{2B2DAE2B-D2BD-4CEC-9894-F229D7042C6D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{0AF45F4B-AC5B-4F95-A797-45443237E702}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
     <workbookView activeTab="5" tabRatio="924" windowHeight="12720" windowWidth="23256" xWindow="-108" xr2:uid="{9831F71E-EE01-4F26-B61E-B641A39E7885}" yWindow="-108"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3772" uniqueCount="1333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3772" uniqueCount="1335">
   <si>
     <t>TestCase_ID</t>
   </si>
@@ -7575,6 +7575,15 @@
     <t>1,174,800.00</t>
   </si>
   <si>
+    <t>08/30/2020</t>
+  </si>
+  <si>
+    <t>07/29/2020</t>
+  </si>
+  <si>
+    <t>Albert Oil Company Inc</t>
+  </si>
+  <si>
     <t>0.0287</t>
   </si>
   <si>
@@ -7629,7 +7638,7 @@
     <t>325.0</t>
   </si>
   <si>
-    <t>2087</t>
+    <t>2094</t>
   </si>
   <si>
     <t>45</t>
@@ -7641,22 +7650,19 @@
     <t>8500</t>
   </si>
   <si>
-    <t>2158.2</t>
-  </si>
-  <si>
-    <t>6.53</t>
-  </si>
-  <si>
-    <t>1901</t>
+    <t>2165.2</t>
+  </si>
+  <si>
+    <t>6.51</t>
+  </si>
+  <si>
+    <t>1902</t>
   </si>
   <si>
     <t>0.12</t>
   </si>
   <si>
-    <t>951 miles in 17 hour(s) 24 minute(s)</t>
-  </si>
-  <si>
-    <t>1900</t>
+    <t>952 miles in 17 hour(s) 29 minute(s)</t>
   </si>
   <si>
     <t>15,625.06</t>
@@ -20096,7 +20102,7 @@
       <pane activePane="bottomRight" state="frozen" topLeftCell="B4" xSplit="1" ySplit="3"/>
       <selection activeCell="B1" pane="topRight" sqref="B1"/>
       <selection activeCell="A4" pane="bottomLeft" sqref="A4"/>
-      <selection activeCell="E11" pane="bottomRight" sqref="E11"/>
+      <selection activeCell="E101" pane="bottomRight" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20340,13 +20346,13 @@
         <v>178</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>890</v>
+        <v>1291</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>890</v>
+        <v>1291</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>890</v>
+        <v>1291</v>
       </c>
     </row>
     <row customHeight="1" ht="18.600000000000001" r="15" spans="2:7" x14ac:dyDescent="0.3">
@@ -20360,13 +20366,13 @@
         <v>226</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>1291</v>
+        <v>1304</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>1291</v>
+        <v>1304</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>1291</v>
+        <v>1304</v>
       </c>
     </row>
     <row customHeight="1" ht="18.600000000000001" r="16" spans="2:7" x14ac:dyDescent="0.3">
@@ -20380,13 +20386,13 @@
         <v>179</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>1292</v>
+        <v>1305</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>1292</v>
+        <v>1305</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>1292</v>
+        <v>1305</v>
       </c>
     </row>
     <row customHeight="1" ht="18.600000000000001" r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -21671,13 +21677,13 @@
         <v>224</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>264</v>
+        <v>1306</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>264</v>
+        <v>1306</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>1306</v>
       </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.3">
@@ -22881,7 +22887,7 @@
       <pane activePane="bottomRight" state="frozen" topLeftCell="B136" xSplit="1" ySplit="3"/>
       <selection activeCell="B1" pane="topRight" sqref="B1"/>
       <selection activeCell="A4" pane="bottomLeft" sqref="A4"/>
-      <selection activeCell="E145" pane="bottomRight" sqref="E145"/>
+      <selection activeCell="E144" pane="bottomRight" sqref="E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23731,13 +23737,13 @@
         <v>560</v>
       </c>
       <c r="E53" t="s">
-        <v>1304</v>
+        <v>1307</v>
       </c>
       <c r="F53" t="s">
-        <v>1304</v>
+        <v>1307</v>
       </c>
       <c r="G53" t="s">
-        <v>1304</v>
+        <v>1307</v>
       </c>
     </row>
     <row customHeight="1" ht="39.6" r="54" spans="2:13" x14ac:dyDescent="0.3">
@@ -23751,13 +23757,13 @@
         <v>561</v>
       </c>
       <c r="E54" t="s">
-        <v>1305</v>
+        <v>1308</v>
       </c>
       <c r="F54" t="s">
-        <v>1305</v>
+        <v>1308</v>
       </c>
       <c r="G54" t="s">
-        <v>1305</v>
+        <v>1308</v>
       </c>
     </row>
     <row customHeight="1" ht="39.6" r="55" spans="2:13" x14ac:dyDescent="0.3">
@@ -23771,13 +23777,13 @@
         <v>562</v>
       </c>
       <c r="E55" t="s">
-        <v>1306</v>
+        <v>1309</v>
       </c>
       <c r="F55" t="s">
-        <v>1306</v>
+        <v>1309</v>
       </c>
       <c r="G55" t="s">
-        <v>1306</v>
+        <v>1309</v>
       </c>
     </row>
     <row customHeight="1" ht="36" r="56" spans="2:13" x14ac:dyDescent="0.3">
@@ -23791,13 +23797,13 @@
         <v>563</v>
       </c>
       <c r="E56" t="s">
-        <v>1307</v>
+        <v>1310</v>
       </c>
       <c r="F56" t="s">
-        <v>1307</v>
+        <v>1310</v>
       </c>
       <c r="G56" t="s">
-        <v>1307</v>
+        <v>1310</v>
       </c>
     </row>
     <row customHeight="1" ht="36" r="57" spans="2:13" x14ac:dyDescent="0.3">
@@ -23811,13 +23817,13 @@
         <v>564</v>
       </c>
       <c r="E57" t="s">
-        <v>1308</v>
+        <v>1311</v>
       </c>
       <c r="F57" t="s">
-        <v>1308</v>
+        <v>1311</v>
       </c>
       <c r="G57" t="s">
-        <v>1308</v>
+        <v>1311</v>
       </c>
     </row>
     <row customHeight="1" ht="36" r="58" spans="2:13" x14ac:dyDescent="0.3">
@@ -23831,13 +23837,13 @@
         <v>565</v>
       </c>
       <c r="E58" t="s">
-        <v>1309</v>
+        <v>1312</v>
       </c>
       <c r="F58" t="s">
-        <v>1309</v>
+        <v>1312</v>
       </c>
       <c r="G58" t="s">
-        <v>1309</v>
+        <v>1312</v>
       </c>
     </row>
     <row customHeight="1" ht="36" r="59" spans="2:13" x14ac:dyDescent="0.3">
@@ -23851,13 +23857,13 @@
         <v>566</v>
       </c>
       <c r="E59" t="s">
-        <v>1310</v>
+        <v>1313</v>
       </c>
       <c r="F59" t="s">
-        <v>1310</v>
+        <v>1313</v>
       </c>
       <c r="G59" t="s">
-        <v>1310</v>
+        <v>1313</v>
       </c>
     </row>
     <row customHeight="1" ht="36" r="60" spans="2:13" x14ac:dyDescent="0.3">
@@ -23891,13 +23897,13 @@
         <v>568</v>
       </c>
       <c r="E61" t="s">
-        <v>1311</v>
+        <v>1314</v>
       </c>
       <c r="F61" t="s">
-        <v>1311</v>
+        <v>1314</v>
       </c>
       <c r="G61" t="s">
-        <v>1311</v>
+        <v>1314</v>
       </c>
     </row>
     <row customHeight="1" ht="58.2" r="62" spans="2:13" x14ac:dyDescent="0.3">
@@ -23922,13 +23928,13 @@
         <v>569</v>
       </c>
       <c r="E63" t="s">
-        <v>1312</v>
+        <v>1315</v>
       </c>
       <c r="F63" t="s">
-        <v>1312</v>
+        <v>1315</v>
       </c>
       <c r="G63" t="s">
-        <v>1312</v>
+        <v>1315</v>
       </c>
     </row>
     <row customHeight="1" ht="26.25" r="64" spans="2:13" x14ac:dyDescent="0.3">
@@ -23942,13 +23948,13 @@
         <v>570</v>
       </c>
       <c r="E64" t="s">
-        <v>1313</v>
+        <v>1316</v>
       </c>
       <c r="F64" t="s">
-        <v>1313</v>
+        <v>1316</v>
       </c>
       <c r="G64" t="s">
-        <v>1313</v>
+        <v>1316</v>
       </c>
     </row>
     <row customHeight="1" ht="24" r="65" spans="2:7" x14ac:dyDescent="0.3">
@@ -23962,13 +23968,13 @@
         <v>571</v>
       </c>
       <c r="E65" t="s">
-        <v>1314</v>
+        <v>1317</v>
       </c>
       <c r="F65" t="s">
-        <v>1314</v>
+        <v>1317</v>
       </c>
       <c r="G65" t="s">
-        <v>1314</v>
+        <v>1317</v>
       </c>
     </row>
     <row customHeight="1" ht="38.4" r="66" spans="2:7" x14ac:dyDescent="0.3">
@@ -23982,13 +23988,13 @@
         <v>575</v>
       </c>
       <c r="E66" t="s">
-        <v>1312</v>
+        <v>1315</v>
       </c>
       <c r="F66" t="s">
-        <v>1312</v>
+        <v>1315</v>
       </c>
       <c r="G66" t="s">
-        <v>1312</v>
+        <v>1315</v>
       </c>
     </row>
     <row customHeight="1" ht="43.8" r="67" spans="2:7" x14ac:dyDescent="0.3">
@@ -24013,13 +24019,13 @@
         <v>572</v>
       </c>
       <c r="E68" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
       <c r="F68" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
       <c r="G68" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
     </row>
     <row customHeight="1" ht="32.4" r="69" spans="2:7" x14ac:dyDescent="0.3">
@@ -24033,13 +24039,13 @@
         <v>573</v>
       </c>
       <c r="E69" t="s">
-        <v>1316</v>
+        <v>1319</v>
       </c>
       <c r="F69" t="s">
-        <v>1316</v>
+        <v>1319</v>
       </c>
       <c r="G69" t="s">
-        <v>1316</v>
+        <v>1319</v>
       </c>
     </row>
     <row customHeight="1" ht="32.4" r="70" spans="2:7" x14ac:dyDescent="0.3">
@@ -24053,13 +24059,13 @@
         <v>574</v>
       </c>
       <c r="E70" t="s">
-        <v>1317</v>
+        <v>1320</v>
       </c>
       <c r="F70" t="s">
-        <v>1317</v>
+        <v>1320</v>
       </c>
       <c r="G70" t="s">
-        <v>1317</v>
+        <v>1320</v>
       </c>
     </row>
     <row customHeight="1" ht="40.799999999999997" r="71" spans="2:7" x14ac:dyDescent="0.3">
@@ -24073,13 +24079,13 @@
         <v>576</v>
       </c>
       <c r="E71" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
       <c r="F71" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
       <c r="G71" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
     </row>
     <row customHeight="1" ht="51" r="72" spans="2:7" x14ac:dyDescent="0.3">
@@ -24104,13 +24110,13 @@
         <v>577</v>
       </c>
       <c r="E73" t="s">
-        <v>1318</v>
+        <v>1321</v>
       </c>
       <c r="F73" t="s">
-        <v>1318</v>
+        <v>1321</v>
       </c>
       <c r="G73" t="s">
-        <v>1318</v>
+        <v>1321</v>
       </c>
     </row>
     <row customHeight="1" ht="34.200000000000003" r="74" spans="2:7" x14ac:dyDescent="0.3">
@@ -24124,13 +24130,13 @@
         <v>578</v>
       </c>
       <c r="E74" t="s">
-        <v>1319</v>
+        <v>1322</v>
       </c>
       <c r="F74" t="s">
-        <v>1319</v>
+        <v>1322</v>
       </c>
       <c r="G74" t="s">
-        <v>1319</v>
+        <v>1322</v>
       </c>
     </row>
     <row customHeight="1" ht="34.200000000000003" r="75" spans="2:7" x14ac:dyDescent="0.3">
@@ -24144,13 +24150,13 @@
         <v>579</v>
       </c>
       <c r="E75" t="s">
-        <v>1320</v>
+        <v>1323</v>
       </c>
       <c r="F75" t="s">
-        <v>1320</v>
+        <v>1323</v>
       </c>
       <c r="G75" t="s">
-        <v>1320</v>
+        <v>1323</v>
       </c>
     </row>
     <row customHeight="1" ht="34.200000000000003" r="76" spans="2:7" x14ac:dyDescent="0.3">
@@ -24164,13 +24170,13 @@
         <v>580</v>
       </c>
       <c r="E76" t="s">
-        <v>1318</v>
+        <v>1321</v>
       </c>
       <c r="F76" t="s">
-        <v>1318</v>
+        <v>1321</v>
       </c>
       <c r="G76" t="s">
-        <v>1318</v>
+        <v>1321</v>
       </c>
     </row>
     <row customHeight="1" ht="52.8" r="77" spans="2:7" x14ac:dyDescent="0.3">
@@ -24725,13 +24731,13 @@
         <v>641</v>
       </c>
       <c r="E123" t="s">
-        <v>1321</v>
+        <v>1324</v>
       </c>
       <c r="F123" t="s">
-        <v>1321</v>
+        <v>1324</v>
       </c>
       <c r="G123" t="s">
-        <v>1321</v>
+        <v>1324</v>
       </c>
     </row>
     <row customHeight="1" ht="29.4" r="124" spans="2:7" x14ac:dyDescent="0.3">
@@ -24745,13 +24751,13 @@
         <v>642</v>
       </c>
       <c r="E124" t="s">
-        <v>1322</v>
+        <v>1325</v>
       </c>
       <c r="F124" t="s">
-        <v>1322</v>
+        <v>1325</v>
       </c>
       <c r="G124" t="s">
-        <v>1322</v>
+        <v>1325</v>
       </c>
     </row>
     <row customHeight="1" ht="29.4" r="125" spans="2:7" x14ac:dyDescent="0.3">
@@ -24765,13 +24771,13 @@
         <v>643</v>
       </c>
       <c r="E125" t="s">
-        <v>1323</v>
+        <v>1326</v>
       </c>
       <c r="F125" t="s">
-        <v>1323</v>
+        <v>1326</v>
       </c>
       <c r="G125" t="s">
-        <v>1323</v>
+        <v>1326</v>
       </c>
     </row>
     <row customHeight="1" ht="29.4" r="126" spans="2:7" x14ac:dyDescent="0.3">
@@ -24785,13 +24791,13 @@
         <v>644</v>
       </c>
       <c r="E126" t="s">
-        <v>1324</v>
+        <v>1327</v>
       </c>
       <c r="F126" t="s">
-        <v>1324</v>
+        <v>1327</v>
       </c>
       <c r="G126" t="s">
-        <v>1324</v>
+        <v>1327</v>
       </c>
     </row>
     <row customHeight="1" ht="29.4" r="127" spans="2:7" x14ac:dyDescent="0.3">
@@ -24805,13 +24811,13 @@
         <v>645</v>
       </c>
       <c r="E127" t="s">
-        <v>1325</v>
+        <v>1328</v>
       </c>
       <c r="F127" t="s">
-        <v>1325</v>
+        <v>1328</v>
       </c>
       <c r="G127" t="s">
-        <v>1325</v>
+        <v>1328</v>
       </c>
     </row>
     <row customHeight="1" ht="29.4" r="128" spans="2:7" x14ac:dyDescent="0.3">
@@ -24825,13 +24831,13 @@
         <v>646</v>
       </c>
       <c r="E128" t="s">
-        <v>1326</v>
+        <v>1329</v>
       </c>
       <c r="F128" t="s">
-        <v>1326</v>
+        <v>1329</v>
       </c>
       <c r="G128" t="s">
-        <v>1326</v>
+        <v>1329</v>
       </c>
     </row>
     <row customHeight="1" ht="29.4" r="129" spans="2:13" x14ac:dyDescent="0.3">
@@ -24845,13 +24851,13 @@
         <v>647</v>
       </c>
       <c r="E129" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
       <c r="F129" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
       <c r="G129" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
     </row>
     <row customHeight="1" ht="29.4" r="130" spans="2:13" x14ac:dyDescent="0.3">
@@ -24865,13 +24871,13 @@
         <v>648</v>
       </c>
       <c r="E130" t="s">
-        <v>1327</v>
+        <v>1330</v>
       </c>
       <c r="F130" t="s">
-        <v>1327</v>
+        <v>1330</v>
       </c>
       <c r="G130" t="s">
-        <v>1327</v>
+        <v>1330</v>
       </c>
     </row>
     <row customHeight="1" ht="29.4" r="131" spans="2:13" x14ac:dyDescent="0.3">
@@ -24885,10 +24891,10 @@
         <v>673</v>
       </c>
       <c r="E131" t="s">
-        <v>1328</v>
+        <v>1331</v>
       </c>
       <c r="F131" t="s">
-        <v>1328</v>
+        <v>1331</v>
       </c>
       <c r="G131" t="s">
         <v>1331</v>
@@ -24905,13 +24911,13 @@
         <v>649</v>
       </c>
       <c r="E132" t="s">
-        <v>1329</v>
+        <v>1332</v>
       </c>
       <c r="F132" t="s">
-        <v>1329</v>
+        <v>1332</v>
       </c>
       <c r="G132" t="s">
-        <v>1329</v>
+        <v>1332</v>
       </c>
     </row>
     <row customHeight="1" ht="29.4" r="133" spans="2:13" x14ac:dyDescent="0.3">
@@ -24925,13 +24931,13 @@
         <v>650</v>
       </c>
       <c r="E133" t="s">
-        <v>1330</v>
+        <v>1333</v>
       </c>
       <c r="F133" t="s">
-        <v>1330</v>
+        <v>1333</v>
       </c>
       <c r="G133" t="s">
-        <v>1330</v>
+        <v>1333</v>
       </c>
     </row>
     <row customHeight="1" ht="56.4" r="134" spans="2:13" x14ac:dyDescent="0.3">
@@ -24956,13 +24962,13 @@
         <v>677</v>
       </c>
       <c r="E135" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
       <c r="F135" t="s">
-        <v>1318</v>
+        <v>1321</v>
       </c>
       <c r="G135" t="s">
-        <v>1332</v>
+        <v>1334</v>
       </c>
       <c r="M135" s="34"/>
     </row>
@@ -24988,13 +24994,13 @@
         <v>679</v>
       </c>
       <c r="E137" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
       <c r="F137" t="s">
-        <v>1318</v>
+        <v>1321</v>
       </c>
       <c r="G137" t="s">
-        <v>1332</v>
+        <v>1334</v>
       </c>
     </row>
     <row customHeight="1" ht="36" r="138" spans="2:13" x14ac:dyDescent="0.3">

</xml_diff>